<commit_message>
Update capabs to point to Jenkins
</commit_message>
<xml_diff>
--- a/src/test/resources/Testdata/TestData.xlsx
+++ b/src/test/resources/Testdata/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\COLLABERA.DIGITAL\eclipse-workspace\AndroidIFiniboAuto\src\test\resources\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BDF3875-E0EB-4DA1-BD37-56F109EA72F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D680E62-6767-409D-9EBC-10B1ABA375E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{597577D0-EBA2-4F46-A758-9A0706E8099C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="511" activeTab="1" xr2:uid="{597577D0-EBA2-4F46-A758-9A0706E8099C}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanAmount" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>Monthly Repayment</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Monthly EMI</t>
+  </si>
+  <si>
+    <t>URL: https://www.calculator.net/auto-loan-calculator.html?csaleprice=1%2C000%2C000&amp;cmonthlypay=750&amp;cloanterm=120&amp;cinterestrate=10&amp;cincentive=0&amp;cdownpayment=100%2C000&amp;ctradeinvalue=0&amp;ctradeinowned=0&amp;cstate=&amp;csaletax=7&amp;ctitlereg=2%2C000&amp;printit=0&amp;ctype=standard&amp;x=Calculate#autoloanresult</t>
   </si>
 </sst>
 </file>
@@ -164,6 +167,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>102740</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>328355</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>573</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5464D9BE-E69E-7AA1-1E57-B780848A35F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="548640" y="3211700"/>
+          <a:ext cx="7864535" cy="6481513"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -938,10 +990,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12300381-93BA-4101-A0BE-544E16C830C8}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1059,24 +1111,24 @@
         <v>3</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="4">
         <f>-PMT(F3%/12,K3,(C3-E3))</f>
-        <v>79124.298507008643</v>
+        <v>11893.566319358548</v>
       </c>
       <c r="K3">
         <f>IF(G3="Years", H3*12, H3 )</f>
-        <v>12</v>
+        <v>120</v>
       </c>
       <c r="L3" s="4">
         <f>-CUMIPMT(F3%/12, K3, (C3-E3), 1, K3,0)</f>
-        <v>49491.58208410372</v>
+        <v>527227.95832302584</v>
       </c>
       <c r="M3" s="4">
         <f>J3*K3</f>
-        <v>949491.58208410372</v>
+        <v>1427227.9583230258</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -1084,7 +1136,6 @@
         <v>3</v>
       </c>
       <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="G4" s="2"/>
       <c r="I4" s="3"/>
@@ -1248,7 +1299,13 @@
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
     </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add screenshot for extentreport
</commit_message>
<xml_diff>
--- a/src/test/resources/Testdata/TestData.xlsx
+++ b/src/test/resources/Testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\COLLABERA.DIGITAL\eclipse-workspace\AndroidIFiniboAuto\src\test\resources\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D680E62-6767-409D-9EBC-10B1ABA375E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5C613C-3C17-4DDF-926D-0B337DEA96F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="511" activeTab="1" xr2:uid="{597577D0-EBA2-4F46-A758-9A0706E8099C}"/>
   </bookViews>
@@ -176,13 +176,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>106680</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>102740</xdr:rowOff>
+      <xdr:rowOff>102741</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>328355</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>573</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>96405</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>83821</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -205,8 +205,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="548640" y="3211700"/>
-          <a:ext cx="7864535" cy="6481513"/>
+          <a:off x="548640" y="3211701"/>
+          <a:ext cx="4858905" cy="4004440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -992,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12300381-93BA-4101-A0BE-544E16C830C8}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add Invalid Test Cases
</commit_message>
<xml_diff>
--- a/src/test/resources/Testdata/TestData.xlsx
+++ b/src/test/resources/Testdata/TestData.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\COLLABERA.DIGITAL\eclipse-workspace\AndroidIFiniboAuto\src\test\resources\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5C613C-3C17-4DDF-926D-0B337DEA96F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B924F202-C758-4793-9048-72351D6C8A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="511" activeTab="1" xr2:uid="{597577D0-EBA2-4F46-A758-9A0706E8099C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="511" activeTab="3" xr2:uid="{597577D0-EBA2-4F46-A758-9A0706E8099C}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanAmount" sheetId="1" r:id="rId1"/>
     <sheet name="VehicleLoan" sheetId="2" r:id="rId2"/>
+    <sheet name="InvalidLoanAmount" sheetId="4" r:id="rId3"/>
+    <sheet name="InvalidVehicleLoan" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="23">
   <si>
     <t>Monthly Repayment</t>
   </si>
@@ -85,6 +87,27 @@
   </si>
   <si>
     <t>URL: https://www.calculator.net/auto-loan-calculator.html?csaleprice=1%2C000%2C000&amp;cmonthlypay=750&amp;cloanterm=120&amp;cinterestrate=10&amp;cincentive=0&amp;cdownpayment=100%2C000&amp;ctradeinvalue=0&amp;ctradeinowned=0&amp;cstate=&amp;csaletax=7&amp;ctitlereg=2%2C000&amp;printit=0&amp;ctype=standard&amp;x=Calculate#autoloanresult</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Invalid Interest Rate</t>
+  </si>
+  <si>
+    <t>Invalid Characters</t>
+  </si>
+  <si>
+    <t>Invalid Loan Term Duration - Years</t>
+  </si>
+  <si>
+    <t>Invalid Loan Term Duration - Months</t>
+  </si>
+  <si>
+    <t>Months</t>
+  </si>
+  <si>
+    <t>InvalidInput</t>
   </si>
 </sst>
 </file>
@@ -992,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12300381-93BA-4101-A0BE-544E16C830C8}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1308,4 +1331,592 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4217A12-8643-471C-977F-E0464CDEBDD9}">
+  <dimension ref="A1:K16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.21875" customWidth="1"/>
+    <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6">
+        <v>10000</v>
+      </c>
+      <c r="D4">
+        <v>101</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6">
+        <v>10000</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>41</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6">
+        <v>10000</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6">
+        <v>481</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="E7" s="2"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="E8" s="2"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="E9" s="2"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="E10" s="2"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="E11" s="2"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="E12" s="2"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="E13" s="2"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="E14" s="2"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="E15" s="2"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="E16" s="2"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8842C00-ABF7-42F8-921E-E28DC5A6AA24}">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4:J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.77734375" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="17.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="G4" s="2"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="G5" s="2"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="G6" s="2"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="G7" s="2"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="G8" s="2"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="G9" s="2"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="G10" s="2"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="G11" s="2"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="G12" s="2"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="G13" s="2"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="G14" s="2"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="G15" s="2"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="G16" s="2"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Invalid Test Cases
</commit_message>
<xml_diff>
--- a/src/test/resources/Testdata/TestData.xlsx
+++ b/src/test/resources/Testdata/TestData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\COLLABERA.DIGITAL\eclipse-workspace\AndroidIFiniboAuto\src\test\resources\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B924F202-C758-4793-9048-72351D6C8A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE818EA-5642-41EB-9EF1-FB869B8D6FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="511" activeTab="3" xr2:uid="{597577D0-EBA2-4F46-A758-9A0706E8099C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="511" activeTab="2" xr2:uid="{597577D0-EBA2-4F46-A758-9A0706E8099C}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanAmount" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="27">
   <si>
     <t>Monthly Repayment</t>
   </si>
@@ -108,6 +108,18 @@
   </si>
   <si>
     <t>InvalidInput</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -546,16 +558,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.21875" customWidth="1"/>
-    <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="4.21875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.5546875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.6640625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.77734375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="23.0"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.44140625"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.88671875"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="17.5546875"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.0"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -1021,14 +1033,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.77734375" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="3.0"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="3.44140625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.6640625"/>
+    <col min="4" max="5" customWidth="true" width="17.77734375"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.77734375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="23.0"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="17.44140625"/>
+    <col min="10" max="13" customWidth="true" width="17.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -1337,22 +1349,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4217A12-8643-471C-977F-E0464CDEBDD9}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.21875" customWidth="1"/>
-    <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="4.21875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.5546875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.6640625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.77734375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="23.0"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.44140625"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="31.33203125"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="17.5546875"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.0"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -1418,8 +1430,8 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="5">
-        <v>2</v>
+      <c r="B3" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>22</v>
@@ -1629,20 +1641,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8842C00-ABF7-42F8-921E-E28DC5A6AA24}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.77734375" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="3.0"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="3.44140625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.6640625"/>
+    <col min="4" max="5" customWidth="true" width="17.77734375"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.77734375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="23.0"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="17.44140625"/>
+    <col min="10" max="13" customWidth="true" width="17.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>